<commit_message>
Added markdown for programming projects
</commit_message>
<xml_diff>
--- a/CV_sections/CV_main.xlsx
+++ b/CV_sections/CV_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/webpage/CV_sections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039A2F38-651E-1648-9AF0-F8C0721FD9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB0C104-FEDF-1E40-BA30-26D72E51D9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="740" windowWidth="29020" windowHeight="16680" activeTab="1" xr2:uid="{C3AA2F21-AFFB-1747-8621-D70A7E3250A3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="en" sheetId="1" r:id="rId1"/>
     <sheet name="fr" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>from</t>
   </si>
@@ -224,6 +224,39 @@
   </si>
   <si>
     <t>Modélisation financière, analyse de données, econometrie</t>
+  </si>
+  <si>
+    <t>Intensive French (A2 → B2)</t>
+  </si>
+  <si>
+    <t>École Suisse International</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>education_other</t>
+  </si>
+  <si>
+    <t>Intensive Latin</t>
+  </si>
+  <si>
+    <t>Harvard Summer School</t>
+  </si>
+  <si>
+    <t>Cambridge, USA</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Français Intensif (A2 / B2)</t>
+  </si>
+  <si>
+    <t>Latin Intensif</t>
+  </si>
+  <si>
+    <t>Cambridge,  États-Unis</t>
   </si>
 </sst>
 </file>
@@ -602,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DFEC79-F959-3C47-94E6-7073962A48B2}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,6 +809,52 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45170</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45261</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="2">
+        <v>41791</v>
+      </c>
+      <c r="F8" s="2">
+        <v>41852</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -783,17 +862,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC5045B-6D00-7E4D-9219-682F636C3EF6}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
-    <col min="7" max="7" width="55.5" customWidth="1"/>
+    <col min="7" max="7" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -955,6 +1034,52 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45170</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45261</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="2">
+        <v>41791</v>
+      </c>
+      <c r="F8" s="2">
+        <v>41852</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>